<commit_message>
Update: Now add new to TPERSON.S10
</commit_message>
<xml_diff>
--- a/s10.xlsx
+++ b/s10.xlsx
@@ -197,20 +197,20 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>使用方法：性别0为男，1为女。起始点设定属性最小值。注意姓名列传都需要使用繁体字，否则会变成空的。
+    <t>王</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>二</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>江</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用方法：性别0为男，1为女。起始点设定属性最小值。注意姓名列传都需要使用繁体字，否则会变成空的。只修改需要自定义的内容即可，其他内容空着默认随机生成。（头像1-774为史实人物，775-884为自定义人物）
 运行s10.exe以后生成的PERSON.S10即自定义武将文件。复制到C:\Users\用户名\Documents\Koei\San10 Tc\TPrsn即可</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>王</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>二</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>江</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -580,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="H5" sqref="A5:XFD5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -593,7 +593,7 @@
   <sheetData>
     <row r="1" spans="1:29" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -750,7 +750,7 @@
       </c>
       <c r="F3" s="2">
         <f ca="1">RANDBETWEEN(1,600)</f>
-        <v>144</v>
+        <v>38</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>33</v>
@@ -766,11 +766,11 @@
       </c>
       <c r="K3" s="2">
         <f ca="1">RANDBETWEEN(1,500)</f>
-        <v>457</v>
+        <v>418</v>
       </c>
       <c r="L3" s="2">
         <f ca="1">RANDBETWEEN(E3,99)</f>
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="M3" s="2">
         <f ca="1">RANDBETWEEN(E3,99)</f>
@@ -778,31 +778,31 @@
       </c>
       <c r="N3" s="2">
         <f ca="1">RANDBETWEEN(E3,99)</f>
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="O3" s="2">
         <f ca="1">RANDBETWEEN(E3,99)</f>
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="P3" s="2">
         <f ca="1">RANDBETWEEN(E3,99)</f>
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Q3" s="2">
         <f ca="1">RANDBETWEEN(0,3)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R3" s="2">
         <f ca="1">RANDBETWEEN(0,2)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S3" s="2">
         <f ca="1">RANDBETWEEN(0,2)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T3" s="2">
         <f ca="1">RANDBETWEEN(0,2)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U3" s="2">
         <v>0</v>
@@ -812,11 +812,11 @@
       </c>
       <c r="W3" s="2">
         <f ca="1">RANDBETWEEN(0,4)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="X3" s="2">
         <f ca="1">RANDBETWEEN(0,4)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y3" s="2">
         <f ca="1">RANDBETWEEN(0,2)</f>
@@ -824,30 +824,30 @@
       </c>
       <c r="Z3" s="2">
         <f ca="1">RANDBETWEEN(0,3)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA3" s="2">
         <f ca="1">RANDBETWEEN(0,3)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AB3" s="2">
         <f ca="1">RANDBETWEEN(0,5)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AC3" s="2">
         <f ca="1">RANDBETWEEN(0,5)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="D4" s="2">
         <v>0</v>
@@ -857,7 +857,7 @@
       </c>
       <c r="F4" s="2">
         <f ca="1">RANDBETWEEN(1,600)</f>
-        <v>154</v>
+        <v>90</v>
       </c>
       <c r="H4" s="2">
         <v>182</v>

</xml_diff>